<commit_message>
Fix Scan and Hello PGN
</commit_message>
<xml_diff>
--- a/Support/PGN 5.6.xlsx
+++ b/Support/PGN 5.6.xlsx
@@ -10,7 +10,7 @@
     <sheet name="PGN" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">PGN!$A$1:$Q$75</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">PGN!$A$1:$Q$86</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="223">
   <si>
     <t>Src</t>
   </si>
@@ -543,15 +543,9 @@
     <t>IP,  MAC</t>
   </si>
   <si>
-    <t>AgIO PGN</t>
-  </si>
-  <si>
     <t>Hello</t>
   </si>
   <si>
-    <t>Version</t>
-  </si>
-  <si>
     <t>Subnet Change</t>
   </si>
   <si>
@@ -622,6 +616,87 @@
   </si>
   <si>
     <t>xte</t>
+  </si>
+  <si>
+    <t>Module ID</t>
+  </si>
+  <si>
+    <t>Machine Reply</t>
+  </si>
+  <si>
+    <t>Steer Reply</t>
+  </si>
+  <si>
+    <t>IMU Reply</t>
+  </si>
+  <si>
+    <t>GPS Reply</t>
+  </si>
+  <si>
+    <t>Subnet Steer</t>
+  </si>
+  <si>
+    <t>Subnet Machine</t>
+  </si>
+  <si>
+    <t>Subnet IMU</t>
+  </si>
+  <si>
+    <t>Subnet GPS</t>
+  </si>
+  <si>
+    <t>ipOne</t>
+  </si>
+  <si>
+    <t>ipTwo</t>
+  </si>
+  <si>
+    <t>ipThree</t>
+  </si>
+  <si>
+    <t>SrcOne</t>
+  </si>
+  <si>
+    <t>SrcTwo</t>
+  </si>
+  <si>
+    <t>SrcThree</t>
+  </si>
+  <si>
+    <t>AngleLo</t>
+  </si>
+  <si>
+    <t>AngleHi</t>
+  </si>
+  <si>
+    <t>CountsLo</t>
+  </si>
+  <si>
+    <t>CountsHi</t>
+  </si>
+  <si>
+    <t>Switchbyte</t>
+  </si>
+  <si>
+    <t>Scan request</t>
+  </si>
+  <si>
+    <t>relayLo</t>
+  </si>
+  <si>
+    <t>relayHi</t>
+  </si>
+  <si>
+    <t>Hello Sent 2 Module</t>
+  </si>
+  <si>
+    <t>From AgIO</t>
+  </si>
+  <si>
+    <t>Subent Reply to AgIO</t>
+  </si>
+  <si>
+    <t>Hello Reply to AgIO</t>
   </si>
 </sst>
 </file>
@@ -973,7 +1048,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1261,6 +1336,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" readingOrder="1"/>
     </xf>
@@ -1278,6 +1359,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="3" borderId="11" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1587,7 +1674,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1598,11 +1685,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:AP74"/>
+  <dimension ref="B1:AP85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N4" sqref="N4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O65" sqref="O65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1759,19 +1846,19 @@
       <c r="H3" s="20">
         <v>8</v>
       </c>
-      <c r="I3" s="101" t="s">
+      <c r="I3" s="103" t="s">
         <v>14</v>
       </c>
-      <c r="J3" s="102"/>
+      <c r="J3" s="104"/>
       <c r="K3" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="L3" s="103" t="s">
+      <c r="L3" s="105" t="s">
         <v>16</v>
       </c>
-      <c r="M3" s="104"/>
+      <c r="M3" s="106"/>
       <c r="N3" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="O3" s="19" t="s">
         <v>18</v>
@@ -1823,10 +1910,10 @@
       <c r="M5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="N5" s="105" t="s">
+      <c r="N5" s="107" t="s">
         <v>34</v>
       </c>
-      <c r="O5" s="105"/>
+      <c r="O5" s="107"/>
       <c r="P5" s="1" t="s">
         <v>35</v>
       </c>
@@ -1915,18 +2002,18 @@
       <c r="H9" s="20">
         <v>8</v>
       </c>
-      <c r="I9" s="106" t="s">
+      <c r="I9" s="108" t="s">
         <v>23</v>
       </c>
-      <c r="J9" s="100"/>
-      <c r="K9" s="105" t="s">
+      <c r="J9" s="102"/>
+      <c r="K9" s="107" t="s">
         <v>24</v>
       </c>
-      <c r="L9" s="105"/>
-      <c r="M9" s="105" t="s">
+      <c r="L9" s="107"/>
+      <c r="M9" s="107" t="s">
         <v>25</v>
       </c>
-      <c r="N9" s="105"/>
+      <c r="N9" s="107"/>
       <c r="O9" s="1" t="s">
         <v>26</v>
       </c>
@@ -2292,7 +2379,7 @@
     <row r="20" spans="2:42" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="11"/>
       <c r="C20" s="58" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D20" s="67" t="s">
         <v>12</v>
@@ -2301,7 +2388,7 @@
         <v>127</v>
       </c>
       <c r="F20" s="48" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G20" s="49">
         <v>235</v>
@@ -2313,100 +2400,100 @@
         <v>1</v>
       </c>
       <c r="J20" s="81" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="K20" s="81">
         <v>2</v>
       </c>
       <c r="L20" s="81" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="M20" s="81">
         <v>3</v>
       </c>
       <c r="N20" s="81" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="O20" s="81">
         <v>4</v>
       </c>
       <c r="P20" s="81" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="Q20" s="81">
         <v>5</v>
       </c>
       <c r="R20" s="92" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="S20" s="92">
         <v>6</v>
       </c>
       <c r="T20" s="92" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="U20" s="92">
         <v>7</v>
       </c>
       <c r="V20" s="92" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="W20" s="92">
         <v>8</v>
       </c>
       <c r="X20" s="92" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="Y20" s="92">
         <v>9</v>
       </c>
       <c r="Z20" s="92" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="AA20" s="92">
         <v>10</v>
       </c>
       <c r="AB20" s="92" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="AC20" s="92">
         <v>11</v>
       </c>
       <c r="AD20" s="92" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="AE20" s="92">
         <v>12</v>
       </c>
       <c r="AF20" s="92" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="AG20" s="92">
         <v>13</v>
       </c>
       <c r="AH20" s="92" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="AI20" s="92">
         <v>14</v>
       </c>
       <c r="AJ20" s="92" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="AK20" s="92">
         <v>15</v>
       </c>
       <c r="AL20" s="92" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="AM20" s="92">
         <v>16</v>
       </c>
       <c r="AN20" s="92" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="AO20" s="3" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="AP20" s="3" t="s">
         <v>20</v>
@@ -2512,18 +2599,18 @@
       <c r="H25" s="20">
         <v>8</v>
       </c>
-      <c r="I25" s="99" t="s">
+      <c r="I25" s="101" t="s">
         <v>132</v>
       </c>
-      <c r="J25" s="100"/>
-      <c r="K25" s="100" t="s">
+      <c r="J25" s="102"/>
+      <c r="K25" s="102" t="s">
         <v>133</v>
       </c>
-      <c r="L25" s="100"/>
-      <c r="M25" s="100" t="s">
+      <c r="L25" s="102"/>
+      <c r="M25" s="102" t="s">
         <v>134</v>
       </c>
-      <c r="N25" s="100"/>
+      <c r="N25" s="102"/>
       <c r="O25" s="20">
         <v>0</v>
       </c>
@@ -3691,10 +3778,10 @@
     </row>
     <row r="61" spans="2:40" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B61" s="90" t="s">
+        <v>219</v>
+      </c>
+      <c r="C61" s="58" t="s">
         <v>171</v>
-      </c>
-      <c r="C61" s="58" t="s">
-        <v>172</v>
       </c>
       <c r="D61" s="67" t="s">
         <v>12</v>
@@ -3708,7 +3795,7 @@
         <v>3</v>
       </c>
       <c r="I61" s="71" t="s">
-        <v>173</v>
+        <v>196</v>
       </c>
       <c r="J61" s="70">
         <v>0</v>
@@ -3748,305 +3835,956 @@
       <c r="AM61" s="91"/>
       <c r="AN61" s="91"/>
     </row>
-    <row r="62" spans="2:40" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B62" s="11"/>
+    <row r="62" spans="2:40" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B62" s="90"/>
       <c r="C62" s="58"/>
       <c r="D62" s="67"/>
       <c r="E62" s="53"/>
       <c r="F62" s="48"/>
       <c r="G62" s="54"/>
-      <c r="H62" s="70"/>
-      <c r="I62" s="71"/>
-      <c r="J62" s="70"/>
-      <c r="K62" s="70"/>
-      <c r="L62" s="70"/>
-      <c r="M62" s="70"/>
-      <c r="N62" s="70"/>
-      <c r="O62" s="70"/>
-      <c r="P62" s="70"/>
-      <c r="Q62" s="70"/>
-      <c r="R62" s="91"/>
-      <c r="S62" s="91"/>
-      <c r="T62" s="91"/>
-      <c r="U62" s="91"/>
-      <c r="V62" s="91"/>
-      <c r="W62" s="91"/>
-      <c r="X62" s="91"/>
-      <c r="Y62" s="91"/>
-      <c r="Z62" s="91"/>
-      <c r="AA62" s="91"/>
-      <c r="AB62" s="91"/>
-      <c r="AC62" s="91"/>
-      <c r="AD62" s="91"/>
-      <c r="AE62" s="91"/>
-      <c r="AF62" s="91"/>
-      <c r="AG62" s="91"/>
-      <c r="AH62" s="91"/>
-      <c r="AI62" s="91"/>
-      <c r="AJ62" s="91"/>
-      <c r="AK62" s="91"/>
-      <c r="AL62" s="91"/>
-      <c r="AM62" s="91"/>
-      <c r="AN62" s="91"/>
-    </row>
-    <row r="63" spans="2:40" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B63" s="11"/>
+      <c r="H62" s="100"/>
+      <c r="I62" s="99"/>
+      <c r="J62" s="100"/>
+      <c r="K62" s="100"/>
+      <c r="L62" s="100"/>
+      <c r="M62" s="100"/>
+      <c r="N62" s="100"/>
+      <c r="O62" s="100"/>
+      <c r="P62" s="100"/>
+      <c r="Q62" s="100"/>
+      <c r="R62" s="100"/>
+      <c r="S62" s="100"/>
+      <c r="T62" s="100"/>
+      <c r="U62" s="100"/>
+      <c r="V62" s="100"/>
+      <c r="W62" s="100"/>
+      <c r="X62" s="100"/>
+      <c r="Y62" s="100"/>
+      <c r="Z62" s="100"/>
+      <c r="AA62" s="100"/>
+      <c r="AB62" s="100"/>
+      <c r="AC62" s="100"/>
+      <c r="AD62" s="100"/>
+      <c r="AE62" s="100"/>
+      <c r="AF62" s="100"/>
+      <c r="AG62" s="100"/>
+      <c r="AH62" s="100"/>
+      <c r="AI62" s="100"/>
+      <c r="AJ62" s="100"/>
+      <c r="AK62" s="100"/>
+      <c r="AL62" s="100"/>
+      <c r="AM62" s="100"/>
+      <c r="AN62" s="100"/>
+    </row>
+    <row r="63" spans="2:40" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B63" s="90" t="s">
+        <v>222</v>
+      </c>
       <c r="C63" s="58" t="s">
-        <v>174</v>
-      </c>
-      <c r="D63" s="67" t="s">
-        <v>12</v>
+        <v>198</v>
+      </c>
+      <c r="D63" s="67">
+        <v>126</v>
       </c>
       <c r="E63" s="53"/>
       <c r="F63" s="48"/>
       <c r="G63" s="54">
-        <v>201</v>
-      </c>
-      <c r="H63" s="70">
+        <v>126</v>
+      </c>
+      <c r="H63" s="100">
         <v>5</v>
       </c>
-      <c r="I63" s="71">
-        <v>201</v>
-      </c>
-      <c r="J63" s="70">
-        <v>201</v>
-      </c>
-      <c r="K63" s="70" t="s">
-        <v>175</v>
-      </c>
-      <c r="L63" s="70" t="s">
-        <v>176</v>
-      </c>
-      <c r="M63" s="70" t="s">
-        <v>177</v>
-      </c>
-      <c r="N63" s="70" t="s">
+      <c r="I63" s="99" t="s">
+        <v>211</v>
+      </c>
+      <c r="J63" s="100" t="s">
+        <v>212</v>
+      </c>
+      <c r="K63" s="100" t="s">
+        <v>213</v>
+      </c>
+      <c r="L63" s="100" t="s">
+        <v>214</v>
+      </c>
+      <c r="M63" s="100" t="s">
+        <v>215</v>
+      </c>
+      <c r="N63" s="100" t="s">
         <v>20</v>
       </c>
-      <c r="O63" s="70"/>
-      <c r="P63" s="70"/>
-      <c r="Q63" s="70"/>
-      <c r="R63" s="91"/>
-      <c r="S63" s="91"/>
-      <c r="T63" s="91"/>
-      <c r="U63" s="91"/>
-      <c r="V63" s="91"/>
-      <c r="W63" s="91"/>
-      <c r="X63" s="91"/>
-      <c r="Y63" s="91"/>
-      <c r="Z63" s="91"/>
-      <c r="AA63" s="91"/>
-      <c r="AB63" s="91"/>
-      <c r="AC63" s="91"/>
-      <c r="AD63" s="91"/>
-      <c r="AE63" s="91"/>
-      <c r="AF63" s="91"/>
-      <c r="AG63" s="91"/>
-      <c r="AH63" s="91"/>
-      <c r="AI63" s="91"/>
-      <c r="AJ63" s="91"/>
-      <c r="AK63" s="91"/>
-      <c r="AL63" s="91"/>
-      <c r="AM63" s="91"/>
-      <c r="AN63" s="91"/>
-    </row>
-    <row r="64" spans="2:40" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B64" s="11"/>
-      <c r="C64" s="58"/>
-      <c r="D64" s="67"/>
+      <c r="O63" s="100"/>
+      <c r="P63" s="100"/>
+      <c r="Q63" s="100"/>
+      <c r="R63" s="100"/>
+      <c r="S63" s="100"/>
+      <c r="T63" s="100"/>
+      <c r="U63" s="100"/>
+      <c r="V63" s="100"/>
+      <c r="W63" s="100"/>
+      <c r="X63" s="100"/>
+      <c r="Y63" s="100"/>
+      <c r="Z63" s="100"/>
+      <c r="AA63" s="100"/>
+      <c r="AB63" s="100"/>
+      <c r="AC63" s="100"/>
+      <c r="AD63" s="100"/>
+      <c r="AE63" s="100"/>
+      <c r="AF63" s="100"/>
+      <c r="AG63" s="100"/>
+      <c r="AH63" s="100"/>
+      <c r="AI63" s="100"/>
+      <c r="AJ63" s="100"/>
+      <c r="AK63" s="100"/>
+      <c r="AL63" s="100"/>
+      <c r="AM63" s="100"/>
+      <c r="AN63" s="100"/>
+    </row>
+    <row r="64" spans="2:40" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B64" s="90"/>
+      <c r="C64" s="58" t="s">
+        <v>197</v>
+      </c>
+      <c r="D64" s="67">
+        <v>123</v>
+      </c>
       <c r="E64" s="53"/>
       <c r="F64" s="48"/>
-      <c r="G64" s="54"/>
-      <c r="H64" s="70"/>
-      <c r="I64" s="71"/>
-      <c r="J64" s="70"/>
-      <c r="K64" s="70"/>
-      <c r="L64" s="70"/>
-      <c r="M64" s="70"/>
-      <c r="N64" s="70"/>
-      <c r="O64" s="70"/>
-      <c r="P64" s="70"/>
-      <c r="Q64" s="70"/>
-      <c r="R64" s="91"/>
-      <c r="S64" s="91"/>
-      <c r="T64" s="91"/>
-      <c r="U64" s="91"/>
-      <c r="V64" s="91"/>
-      <c r="W64" s="91"/>
-      <c r="X64" s="91"/>
-      <c r="Y64" s="91"/>
-      <c r="Z64" s="91"/>
-      <c r="AA64" s="91"/>
-      <c r="AB64" s="91"/>
-      <c r="AC64" s="91"/>
-      <c r="AD64" s="91"/>
-      <c r="AE64" s="91"/>
-      <c r="AF64" s="91"/>
-      <c r="AG64" s="91"/>
-      <c r="AH64" s="91"/>
-      <c r="AI64" s="91"/>
-      <c r="AJ64" s="91"/>
-      <c r="AK64" s="91"/>
-      <c r="AL64" s="91"/>
-      <c r="AM64" s="91"/>
-      <c r="AN64" s="91"/>
-    </row>
-    <row r="65" spans="2:40" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B65" s="11"/>
-      <c r="C65" s="58"/>
-      <c r="D65" s="67"/>
+      <c r="G64" s="54">
+        <v>123</v>
+      </c>
+      <c r="H64" s="100">
+        <v>5</v>
+      </c>
+      <c r="I64" s="99" t="s">
+        <v>217</v>
+      </c>
+      <c r="J64" s="100" t="s">
+        <v>218</v>
+      </c>
+      <c r="K64" s="100" t="s">
+        <v>67</v>
+      </c>
+      <c r="L64" s="100" t="s">
+        <v>67</v>
+      </c>
+      <c r="M64" s="100" t="s">
+        <v>67</v>
+      </c>
+      <c r="N64" s="100" t="s">
+        <v>20</v>
+      </c>
+      <c r="O64" s="100"/>
+      <c r="P64" s="100"/>
+      <c r="Q64" s="100"/>
+      <c r="R64" s="100"/>
+      <c r="S64" s="100"/>
+      <c r="T64" s="100"/>
+      <c r="U64" s="100"/>
+      <c r="V64" s="100"/>
+      <c r="W64" s="100"/>
+      <c r="X64" s="100"/>
+      <c r="Y64" s="100"/>
+      <c r="Z64" s="100"/>
+      <c r="AA64" s="100"/>
+      <c r="AB64" s="100"/>
+      <c r="AC64" s="100"/>
+      <c r="AD64" s="100"/>
+      <c r="AE64" s="100"/>
+      <c r="AF64" s="100"/>
+      <c r="AG64" s="100"/>
+      <c r="AH64" s="100"/>
+      <c r="AI64" s="100"/>
+      <c r="AJ64" s="100"/>
+      <c r="AK64" s="100"/>
+      <c r="AL64" s="100"/>
+      <c r="AM64" s="100"/>
+      <c r="AN64" s="100"/>
+    </row>
+    <row r="65" spans="2:40" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B65" s="90"/>
+      <c r="C65" s="58" t="s">
+        <v>199</v>
+      </c>
+      <c r="D65" s="67">
+        <v>121</v>
+      </c>
       <c r="E65" s="53"/>
       <c r="F65" s="48"/>
-      <c r="G65" s="54"/>
-      <c r="H65" s="70"/>
-      <c r="I65" s="71"/>
-      <c r="J65" s="70"/>
-      <c r="K65" s="70"/>
-      <c r="L65" s="70"/>
-      <c r="M65" s="70"/>
-      <c r="N65" s="70"/>
-      <c r="O65" s="70"/>
-      <c r="P65" s="70"/>
-      <c r="Q65" s="70"/>
-      <c r="R65" s="91"/>
-      <c r="S65" s="91"/>
-      <c r="T65" s="91"/>
-      <c r="U65" s="91"/>
-      <c r="V65" s="91"/>
-      <c r="W65" s="91"/>
-      <c r="X65" s="91"/>
-      <c r="Y65" s="91"/>
-      <c r="Z65" s="91"/>
-      <c r="AA65" s="91"/>
-      <c r="AB65" s="91"/>
-      <c r="AC65" s="91"/>
-      <c r="AD65" s="91"/>
-      <c r="AE65" s="91"/>
-      <c r="AF65" s="91"/>
-      <c r="AG65" s="91"/>
-      <c r="AH65" s="91"/>
-      <c r="AI65" s="91"/>
-      <c r="AJ65" s="91"/>
-      <c r="AK65" s="91"/>
-      <c r="AL65" s="91"/>
-      <c r="AM65" s="91"/>
-      <c r="AN65" s="91"/>
-    </row>
-    <row r="66" spans="2:40" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="67" spans="2:40" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C67" s="78" t="s">
+      <c r="G65" s="54">
+        <v>121</v>
+      </c>
+      <c r="H65" s="100">
+        <v>5</v>
+      </c>
+      <c r="I65" s="99" t="s">
+        <v>67</v>
+      </c>
+      <c r="J65" s="99" t="s">
+        <v>67</v>
+      </c>
+      <c r="K65" s="99" t="s">
+        <v>67</v>
+      </c>
+      <c r="L65" s="99" t="s">
+        <v>67</v>
+      </c>
+      <c r="M65" s="99" t="s">
+        <v>67</v>
+      </c>
+      <c r="N65" s="100" t="s">
+        <v>20</v>
+      </c>
+      <c r="O65" s="100"/>
+      <c r="P65" s="100"/>
+      <c r="Q65" s="100"/>
+      <c r="R65" s="100"/>
+      <c r="S65" s="100"/>
+      <c r="T65" s="100"/>
+      <c r="U65" s="100"/>
+      <c r="V65" s="100"/>
+      <c r="W65" s="100"/>
+      <c r="X65" s="100"/>
+      <c r="Y65" s="100"/>
+      <c r="Z65" s="100"/>
+      <c r="AA65" s="100"/>
+      <c r="AB65" s="100"/>
+      <c r="AC65" s="100"/>
+      <c r="AD65" s="100"/>
+      <c r="AE65" s="100"/>
+      <c r="AF65" s="100"/>
+      <c r="AG65" s="100"/>
+      <c r="AH65" s="100"/>
+      <c r="AI65" s="100"/>
+      <c r="AJ65" s="100"/>
+      <c r="AK65" s="100"/>
+      <c r="AL65" s="100"/>
+      <c r="AM65" s="100"/>
+      <c r="AN65" s="100"/>
+    </row>
+    <row r="66" spans="2:40" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B66" s="90"/>
+      <c r="C66" s="58" t="s">
+        <v>200</v>
+      </c>
+      <c r="D66" s="67">
+        <v>120</v>
+      </c>
+      <c r="E66" s="53"/>
+      <c r="F66" s="48"/>
+      <c r="G66" s="54">
+        <v>120</v>
+      </c>
+      <c r="H66" s="100">
+        <v>5</v>
+      </c>
+      <c r="I66" s="99" t="s">
+        <v>67</v>
+      </c>
+      <c r="J66" s="99" t="s">
+        <v>67</v>
+      </c>
+      <c r="K66" s="99" t="s">
+        <v>67</v>
+      </c>
+      <c r="L66" s="99" t="s">
+        <v>67</v>
+      </c>
+      <c r="M66" s="99" t="s">
+        <v>67</v>
+      </c>
+      <c r="N66" s="100" t="s">
+        <v>20</v>
+      </c>
+      <c r="O66" s="100"/>
+      <c r="P66" s="100"/>
+      <c r="Q66" s="100"/>
+      <c r="R66" s="100"/>
+      <c r="S66" s="100"/>
+      <c r="T66" s="100"/>
+      <c r="U66" s="100"/>
+      <c r="V66" s="100"/>
+      <c r="W66" s="100"/>
+      <c r="X66" s="100"/>
+      <c r="Y66" s="100"/>
+      <c r="Z66" s="100"/>
+      <c r="AA66" s="100"/>
+      <c r="AB66" s="100"/>
+      <c r="AC66" s="100"/>
+      <c r="AD66" s="100"/>
+      <c r="AE66" s="100"/>
+      <c r="AF66" s="100"/>
+      <c r="AG66" s="100"/>
+      <c r="AH66" s="100"/>
+      <c r="AI66" s="100"/>
+      <c r="AJ66" s="100"/>
+      <c r="AK66" s="100"/>
+      <c r="AL66" s="100"/>
+      <c r="AM66" s="100"/>
+      <c r="AN66" s="100"/>
+    </row>
+    <row r="67" spans="2:40" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B67" s="11"/>
+      <c r="C67" s="58"/>
+      <c r="D67" s="67"/>
+      <c r="E67" s="53"/>
+      <c r="F67" s="48"/>
+      <c r="G67" s="54"/>
+      <c r="H67" s="70"/>
+      <c r="I67" s="71"/>
+      <c r="J67" s="70"/>
+      <c r="K67" s="70"/>
+      <c r="L67" s="70"/>
+      <c r="M67" s="70"/>
+      <c r="N67" s="70"/>
+      <c r="O67" s="70"/>
+      <c r="P67" s="70"/>
+      <c r="Q67" s="70"/>
+      <c r="R67" s="91"/>
+      <c r="S67" s="91"/>
+      <c r="T67" s="91"/>
+      <c r="U67" s="91"/>
+      <c r="V67" s="91"/>
+      <c r="W67" s="91"/>
+      <c r="X67" s="91"/>
+      <c r="Y67" s="91"/>
+      <c r="Z67" s="91"/>
+      <c r="AA67" s="91"/>
+      <c r="AB67" s="91"/>
+      <c r="AC67" s="91"/>
+      <c r="AD67" s="91"/>
+      <c r="AE67" s="91"/>
+      <c r="AF67" s="91"/>
+      <c r="AG67" s="91"/>
+      <c r="AH67" s="91"/>
+      <c r="AI67" s="91"/>
+      <c r="AJ67" s="91"/>
+      <c r="AK67" s="91"/>
+      <c r="AL67" s="91"/>
+      <c r="AM67" s="91"/>
+      <c r="AN67" s="91"/>
+    </row>
+    <row r="68" spans="2:40" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B68" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="C68" s="58" t="s">
+        <v>172</v>
+      </c>
+      <c r="D68" s="67" t="s">
+        <v>12</v>
+      </c>
+      <c r="E68" s="53"/>
+      <c r="F68" s="48"/>
+      <c r="G68" s="54">
+        <v>201</v>
+      </c>
+      <c r="H68" s="70">
+        <v>5</v>
+      </c>
+      <c r="I68" s="71">
+        <v>201</v>
+      </c>
+      <c r="J68" s="70">
+        <v>201</v>
+      </c>
+      <c r="K68" s="70" t="s">
+        <v>173</v>
+      </c>
+      <c r="L68" s="70" t="s">
+        <v>174</v>
+      </c>
+      <c r="M68" s="70" t="s">
+        <v>175</v>
+      </c>
+      <c r="N68" s="70" t="s">
+        <v>20</v>
+      </c>
+      <c r="O68" s="70"/>
+      <c r="P68" s="70"/>
+      <c r="Q68" s="70"/>
+      <c r="R68" s="91"/>
+      <c r="S68" s="91"/>
+      <c r="T68" s="91"/>
+      <c r="U68" s="91"/>
+      <c r="V68" s="91"/>
+      <c r="W68" s="91"/>
+      <c r="X68" s="91"/>
+      <c r="Y68" s="91"/>
+      <c r="Z68" s="91"/>
+      <c r="AA68" s="91"/>
+      <c r="AB68" s="91"/>
+      <c r="AC68" s="91"/>
+      <c r="AD68" s="91"/>
+      <c r="AE68" s="91"/>
+      <c r="AF68" s="91"/>
+      <c r="AG68" s="91"/>
+      <c r="AH68" s="91"/>
+      <c r="AI68" s="91"/>
+      <c r="AJ68" s="91"/>
+      <c r="AK68" s="91"/>
+      <c r="AL68" s="91"/>
+      <c r="AM68" s="91"/>
+      <c r="AN68" s="91"/>
+    </row>
+    <row r="69" spans="2:40" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B69" s="11"/>
+      <c r="C69" s="58"/>
+      <c r="D69" s="67"/>
+      <c r="E69" s="53"/>
+      <c r="F69" s="48"/>
+      <c r="G69" s="54"/>
+      <c r="H69" s="100"/>
+      <c r="I69" s="99"/>
+      <c r="J69" s="100"/>
+      <c r="K69" s="100"/>
+      <c r="L69" s="100"/>
+      <c r="M69" s="100"/>
+      <c r="N69" s="100"/>
+      <c r="O69" s="100"/>
+      <c r="P69" s="100"/>
+      <c r="Q69" s="100"/>
+      <c r="R69" s="100"/>
+      <c r="S69" s="100"/>
+      <c r="T69" s="100"/>
+      <c r="U69" s="100"/>
+      <c r="V69" s="100"/>
+      <c r="W69" s="100"/>
+      <c r="X69" s="100"/>
+      <c r="Y69" s="100"/>
+      <c r="Z69" s="100"/>
+      <c r="AA69" s="100"/>
+      <c r="AB69" s="100"/>
+      <c r="AC69" s="100"/>
+      <c r="AD69" s="100"/>
+      <c r="AE69" s="100"/>
+      <c r="AF69" s="100"/>
+      <c r="AG69" s="100"/>
+      <c r="AH69" s="100"/>
+      <c r="AI69" s="100"/>
+      <c r="AJ69" s="100"/>
+      <c r="AK69" s="100"/>
+      <c r="AL69" s="100"/>
+      <c r="AM69" s="100"/>
+      <c r="AN69" s="100"/>
+    </row>
+    <row r="70" spans="2:40" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B70" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="C70" s="110" t="s">
+        <v>216</v>
+      </c>
+      <c r="D70" s="67" t="s">
+        <v>12</v>
+      </c>
+      <c r="E70" s="53"/>
+      <c r="F70" s="48"/>
+      <c r="G70" s="54">
+        <v>202</v>
+      </c>
+      <c r="H70" s="70">
+        <v>3</v>
+      </c>
+      <c r="I70" s="71">
+        <v>202</v>
+      </c>
+      <c r="J70" s="70">
+        <v>202</v>
+      </c>
+      <c r="K70" s="70">
+        <v>5</v>
+      </c>
+      <c r="L70" s="70" t="s">
+        <v>20</v>
+      </c>
+      <c r="M70" s="70"/>
+      <c r="N70" s="70"/>
+      <c r="O70" s="70"/>
+      <c r="P70" s="70"/>
+      <c r="Q70" s="70"/>
+      <c r="R70" s="91"/>
+      <c r="S70" s="91"/>
+      <c r="T70" s="91"/>
+      <c r="U70" s="91"/>
+      <c r="V70" s="91"/>
+      <c r="W70" s="91"/>
+      <c r="X70" s="91"/>
+      <c r="Y70" s="91"/>
+      <c r="Z70" s="91"/>
+      <c r="AA70" s="91"/>
+      <c r="AB70" s="91"/>
+      <c r="AC70" s="91"/>
+      <c r="AD70" s="91"/>
+      <c r="AE70" s="91"/>
+      <c r="AF70" s="91"/>
+      <c r="AG70" s="91"/>
+      <c r="AH70" s="91"/>
+      <c r="AI70" s="91"/>
+      <c r="AJ70" s="91"/>
+      <c r="AK70" s="91"/>
+      <c r="AL70" s="91"/>
+      <c r="AM70" s="91"/>
+      <c r="AN70" s="91"/>
+    </row>
+    <row r="71" spans="2:40" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B71" s="11"/>
+      <c r="C71" s="110"/>
+      <c r="D71" s="67"/>
+      <c r="E71" s="53"/>
+      <c r="F71" s="48"/>
+      <c r="G71" s="54"/>
+      <c r="H71" s="100"/>
+      <c r="I71" s="99"/>
+      <c r="J71" s="100"/>
+      <c r="K71" s="100"/>
+      <c r="L71" s="100"/>
+      <c r="M71" s="100"/>
+      <c r="N71" s="100"/>
+      <c r="O71" s="100"/>
+      <c r="P71" s="100"/>
+      <c r="Q71" s="100"/>
+      <c r="R71" s="100"/>
+      <c r="S71" s="100"/>
+      <c r="T71" s="100"/>
+      <c r="U71" s="100"/>
+      <c r="V71" s="100"/>
+      <c r="W71" s="100"/>
+      <c r="X71" s="100"/>
+      <c r="Y71" s="100"/>
+      <c r="Z71" s="100"/>
+      <c r="AA71" s="100"/>
+      <c r="AB71" s="100"/>
+      <c r="AC71" s="100"/>
+      <c r="AD71" s="100"/>
+      <c r="AE71" s="100"/>
+      <c r="AF71" s="100"/>
+      <c r="AG71" s="100"/>
+      <c r="AH71" s="100"/>
+      <c r="AI71" s="100"/>
+      <c r="AJ71" s="100"/>
+      <c r="AK71" s="100"/>
+      <c r="AL71" s="100"/>
+      <c r="AM71" s="100"/>
+      <c r="AN71" s="100"/>
+    </row>
+    <row r="72" spans="2:40" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B72" s="11" t="s">
+        <v>221</v>
+      </c>
+      <c r="C72" s="58" t="s">
+        <v>201</v>
+      </c>
+      <c r="D72" s="109">
+        <v>126</v>
+      </c>
+      <c r="E72" s="53"/>
+      <c r="F72" s="48"/>
+      <c r="G72" s="54">
+        <v>203</v>
+      </c>
+      <c r="H72" s="70">
+        <v>7</v>
+      </c>
+      <c r="I72" s="71" t="s">
+        <v>205</v>
+      </c>
+      <c r="J72" s="70" t="s">
+        <v>206</v>
+      </c>
+      <c r="K72" s="70" t="s">
+        <v>207</v>
+      </c>
+      <c r="L72" s="70">
+        <v>126</v>
+      </c>
+      <c r="M72" s="70" t="s">
+        <v>208</v>
+      </c>
+      <c r="N72" s="70" t="s">
+        <v>209</v>
+      </c>
+      <c r="O72" s="70" t="s">
+        <v>210</v>
+      </c>
+      <c r="P72" s="70" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q72" s="70"/>
+      <c r="R72" s="91"/>
+      <c r="S72" s="91"/>
+      <c r="T72" s="91"/>
+      <c r="U72" s="91"/>
+      <c r="V72" s="91"/>
+      <c r="W72" s="91"/>
+      <c r="X72" s="91"/>
+      <c r="Y72" s="91"/>
+      <c r="Z72" s="91"/>
+      <c r="AA72" s="91"/>
+      <c r="AB72" s="91"/>
+      <c r="AC72" s="91"/>
+      <c r="AD72" s="91"/>
+      <c r="AE72" s="91"/>
+      <c r="AF72" s="91"/>
+      <c r="AG72" s="91"/>
+      <c r="AH72" s="91"/>
+      <c r="AI72" s="91"/>
+      <c r="AJ72" s="91"/>
+      <c r="AK72" s="91"/>
+      <c r="AL72" s="91"/>
+      <c r="AM72" s="91"/>
+      <c r="AN72" s="91"/>
+    </row>
+    <row r="73" spans="2:40" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B73" s="11"/>
+      <c r="C73" s="58" t="s">
+        <v>202</v>
+      </c>
+      <c r="D73" s="109">
+        <v>123</v>
+      </c>
+      <c r="E73" s="53"/>
+      <c r="F73" s="48"/>
+      <c r="G73" s="54">
+        <v>203</v>
+      </c>
+      <c r="H73" s="100">
+        <v>7</v>
+      </c>
+      <c r="I73" s="99" t="s">
+        <v>205</v>
+      </c>
+      <c r="J73" s="100" t="s">
+        <v>206</v>
+      </c>
+      <c r="K73" s="100" t="s">
+        <v>207</v>
+      </c>
+      <c r="L73" s="100">
+        <v>123</v>
+      </c>
+      <c r="M73" s="100" t="s">
+        <v>208</v>
+      </c>
+      <c r="N73" s="100" t="s">
+        <v>209</v>
+      </c>
+      <c r="O73" s="100" t="s">
+        <v>210</v>
+      </c>
+      <c r="P73" s="100" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q73" s="100"/>
+      <c r="R73" s="100"/>
+      <c r="S73" s="100"/>
+      <c r="T73" s="100"/>
+      <c r="U73" s="100"/>
+      <c r="V73" s="100"/>
+      <c r="W73" s="100"/>
+      <c r="X73" s="100"/>
+      <c r="Y73" s="100"/>
+      <c r="Z73" s="100"/>
+      <c r="AA73" s="100"/>
+      <c r="AB73" s="100"/>
+      <c r="AC73" s="100"/>
+      <c r="AD73" s="100"/>
+      <c r="AE73" s="100"/>
+      <c r="AF73" s="100"/>
+      <c r="AG73" s="100"/>
+      <c r="AH73" s="100"/>
+      <c r="AI73" s="100"/>
+      <c r="AJ73" s="100"/>
+      <c r="AK73" s="100"/>
+      <c r="AL73" s="100"/>
+      <c r="AM73" s="100"/>
+      <c r="AN73" s="100"/>
+    </row>
+    <row r="74" spans="2:40" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B74" s="11"/>
+      <c r="C74" s="58" t="s">
+        <v>203</v>
+      </c>
+      <c r="D74" s="109">
+        <v>121</v>
+      </c>
+      <c r="E74" s="53"/>
+      <c r="F74" s="48"/>
+      <c r="G74" s="54">
+        <v>203</v>
+      </c>
+      <c r="H74" s="100">
+        <v>7</v>
+      </c>
+      <c r="I74" s="99" t="s">
+        <v>205</v>
+      </c>
+      <c r="J74" s="100" t="s">
+        <v>206</v>
+      </c>
+      <c r="K74" s="100" t="s">
+        <v>207</v>
+      </c>
+      <c r="L74" s="100">
+        <v>121</v>
+      </c>
+      <c r="M74" s="100" t="s">
+        <v>208</v>
+      </c>
+      <c r="N74" s="100" t="s">
+        <v>209</v>
+      </c>
+      <c r="O74" s="100" t="s">
+        <v>210</v>
+      </c>
+      <c r="P74" s="100" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q74" s="100"/>
+      <c r="R74" s="100"/>
+      <c r="S74" s="100"/>
+      <c r="T74" s="100"/>
+      <c r="U74" s="100"/>
+      <c r="V74" s="100"/>
+      <c r="W74" s="100"/>
+      <c r="X74" s="100"/>
+      <c r="Y74" s="100"/>
+      <c r="Z74" s="100"/>
+      <c r="AA74" s="100"/>
+      <c r="AB74" s="100"/>
+      <c r="AC74" s="100"/>
+      <c r="AD74" s="100"/>
+      <c r="AE74" s="100"/>
+      <c r="AF74" s="100"/>
+      <c r="AG74" s="100"/>
+      <c r="AH74" s="100"/>
+      <c r="AI74" s="100"/>
+      <c r="AJ74" s="100"/>
+      <c r="AK74" s="100"/>
+      <c r="AL74" s="100"/>
+      <c r="AM74" s="100"/>
+      <c r="AN74" s="100"/>
+    </row>
+    <row r="75" spans="2:40" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B75" s="11"/>
+      <c r="C75" s="58" t="s">
+        <v>204</v>
+      </c>
+      <c r="D75" s="109">
+        <v>120</v>
+      </c>
+      <c r="E75" s="53"/>
+      <c r="F75" s="48"/>
+      <c r="G75" s="54">
+        <v>203</v>
+      </c>
+      <c r="H75" s="100">
+        <v>7</v>
+      </c>
+      <c r="I75" s="99" t="s">
+        <v>205</v>
+      </c>
+      <c r="J75" s="100" t="s">
+        <v>206</v>
+      </c>
+      <c r="K75" s="100" t="s">
+        <v>207</v>
+      </c>
+      <c r="L75" s="100">
+        <v>120</v>
+      </c>
+      <c r="M75" s="100" t="s">
+        <v>208</v>
+      </c>
+      <c r="N75" s="100" t="s">
+        <v>209</v>
+      </c>
+      <c r="O75" s="100" t="s">
+        <v>210</v>
+      </c>
+      <c r="P75" s="100" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q75" s="100"/>
+      <c r="R75" s="100"/>
+      <c r="S75" s="100"/>
+      <c r="T75" s="100"/>
+      <c r="U75" s="100"/>
+      <c r="V75" s="100"/>
+      <c r="W75" s="100"/>
+      <c r="X75" s="100"/>
+      <c r="Y75" s="100"/>
+      <c r="Z75" s="100"/>
+      <c r="AA75" s="100"/>
+      <c r="AB75" s="100"/>
+      <c r="AC75" s="100"/>
+      <c r="AD75" s="100"/>
+      <c r="AE75" s="100"/>
+      <c r="AF75" s="100"/>
+      <c r="AG75" s="100"/>
+      <c r="AH75" s="100"/>
+      <c r="AI75" s="100"/>
+      <c r="AJ75" s="100"/>
+      <c r="AK75" s="100"/>
+      <c r="AL75" s="100"/>
+      <c r="AM75" s="100"/>
+      <c r="AN75" s="100"/>
+    </row>
+    <row r="76" spans="2:40" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B76" s="11"/>
+      <c r="C76" s="58"/>
+      <c r="D76" s="109"/>
+      <c r="E76" s="53"/>
+      <c r="F76" s="48"/>
+      <c r="G76" s="54"/>
+      <c r="H76" s="100"/>
+      <c r="I76" s="99"/>
+      <c r="J76" s="100"/>
+      <c r="K76" s="100"/>
+      <c r="L76" s="100"/>
+      <c r="M76" s="100"/>
+      <c r="N76" s="100"/>
+      <c r="O76" s="100"/>
+      <c r="P76" s="100"/>
+      <c r="Q76" s="100"/>
+      <c r="R76" s="100"/>
+      <c r="S76" s="100"/>
+      <c r="T76" s="100"/>
+      <c r="U76" s="100"/>
+      <c r="V76" s="100"/>
+      <c r="W76" s="100"/>
+      <c r="X76" s="100"/>
+      <c r="Y76" s="100"/>
+      <c r="Z76" s="100"/>
+      <c r="AA76" s="100"/>
+      <c r="AB76" s="100"/>
+      <c r="AC76" s="100"/>
+      <c r="AD76" s="100"/>
+      <c r="AE76" s="100"/>
+      <c r="AF76" s="100"/>
+      <c r="AG76" s="100"/>
+      <c r="AH76" s="100"/>
+      <c r="AI76" s="100"/>
+      <c r="AJ76" s="100"/>
+      <c r="AK76" s="100"/>
+      <c r="AL76" s="100"/>
+      <c r="AM76" s="100"/>
+      <c r="AN76" s="100"/>
+    </row>
+    <row r="77" spans="2:40" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="78" spans="2:40" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C78" s="78" t="s">
         <v>170</v>
       </c>
-      <c r="D67" s="74" t="s">
+      <c r="D78" s="74" t="s">
         <v>169</v>
       </c>
-      <c r="E67" s="75"/>
-      <c r="F67" s="76" t="s">
+      <c r="E78" s="75"/>
+      <c r="F78" s="76" t="s">
         <v>168</v>
       </c>
-      <c r="G67" s="77"/>
-    </row>
-    <row r="68" spans="2:40" x14ac:dyDescent="0.2">
-      <c r="B68" s="73" t="s">
+      <c r="G78" s="77"/>
+    </row>
+    <row r="79" spans="2:40" x14ac:dyDescent="0.2">
+      <c r="B79" s="73" t="s">
         <v>136</v>
       </c>
-      <c r="C68" s="72" t="s">
+      <c r="C79" s="72" t="s">
         <v>165</v>
       </c>
-      <c r="D68" s="67">
+      <c r="D79" s="67">
         <v>254</v>
       </c>
-      <c r="E68" s="47" t="s">
+      <c r="E79" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="F68" s="48">
+      <c r="F79" s="48">
         <v>253</v>
       </c>
-      <c r="G68" s="49" t="s">
+      <c r="G79" s="49" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="69" spans="2:40" x14ac:dyDescent="0.2">
-      <c r="B69" s="73"/>
-      <c r="C69" s="72"/>
-      <c r="H69" s="22"/>
-      <c r="I69" s="27"/>
-      <c r="J69" s="21"/>
-      <c r="K69" s="21"/>
-      <c r="L69" s="21"/>
-      <c r="M69" s="21"/>
-      <c r="N69" s="21"/>
-      <c r="O69" s="21"/>
-      <c r="P69" s="21"/>
-      <c r="Q69" s="21"/>
-    </row>
-    <row r="70" spans="2:40" x14ac:dyDescent="0.2">
-      <c r="B70" s="73" t="s">
+    <row r="80" spans="2:40" x14ac:dyDescent="0.2">
+      <c r="B80" s="73"/>
+      <c r="C80" s="72"/>
+      <c r="H80" s="22"/>
+      <c r="I80" s="27"/>
+      <c r="J80" s="21"/>
+      <c r="K80" s="21"/>
+      <c r="L80" s="21"/>
+      <c r="M80" s="21"/>
+      <c r="N80" s="21"/>
+      <c r="O80" s="21"/>
+      <c r="P80" s="21"/>
+      <c r="Q80" s="21"/>
+    </row>
+    <row r="81" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B81" s="73" t="s">
         <v>137</v>
       </c>
-      <c r="C70" s="72" t="s">
+      <c r="C81" s="72" t="s">
         <v>164</v>
       </c>
-      <c r="D70" s="67">
+      <c r="D81" s="67">
         <v>239</v>
       </c>
-      <c r="E70" s="47" t="s">
+      <c r="E81" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="F70" s="48">
+      <c r="F81" s="48">
         <v>237</v>
       </c>
-      <c r="G70" s="49" t="s">
+      <c r="G81" s="49" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="71" spans="2:40" x14ac:dyDescent="0.2">
-      <c r="B71" s="73"/>
-      <c r="C71" s="72"/>
-      <c r="H71" s="22"/>
-      <c r="I71" s="27"/>
-      <c r="J71" s="21"/>
-      <c r="K71" s="21"/>
-      <c r="L71" s="21"/>
-      <c r="M71" s="21"/>
-      <c r="N71" s="21"/>
-      <c r="O71" s="21"/>
-      <c r="P71" s="21"/>
-      <c r="Q71" s="21"/>
-    </row>
-    <row r="72" spans="2:40" x14ac:dyDescent="0.2">
-      <c r="B72" s="73" t="s">
+    <row r="82" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B82" s="73"/>
+      <c r="C82" s="72"/>
+      <c r="H82" s="22"/>
+      <c r="I82" s="27"/>
+      <c r="J82" s="21"/>
+      <c r="K82" s="21"/>
+      <c r="L82" s="21"/>
+      <c r="M82" s="21"/>
+      <c r="N82" s="21"/>
+      <c r="O82" s="21"/>
+      <c r="P82" s="21"/>
+      <c r="Q82" s="21"/>
+    </row>
+    <row r="83" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B83" s="73" t="s">
         <v>59</v>
       </c>
-      <c r="C72" s="72" t="s">
+      <c r="C83" s="72" t="s">
         <v>166</v>
       </c>
-      <c r="F72" s="48">
+      <c r="F83" s="48">
         <v>211</v>
       </c>
-      <c r="G72" s="49" t="s">
+      <c r="G83" s="49" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="73" spans="2:40" x14ac:dyDescent="0.2">
-      <c r="B73" s="73"/>
-      <c r="C73" s="72"/>
-      <c r="H73" s="22"/>
-      <c r="I73" s="27"/>
-      <c r="J73" s="21"/>
-      <c r="K73" s="21"/>
-      <c r="L73" s="21"/>
-      <c r="M73" s="21"/>
-      <c r="N73" s="21"/>
-      <c r="O73" s="21"/>
-      <c r="P73" s="21"/>
-      <c r="Q73" s="21"/>
-    </row>
-    <row r="74" spans="2:40" x14ac:dyDescent="0.2">
-      <c r="B74" s="73" t="s">
+    <row r="84" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B84" s="73"/>
+      <c r="C84" s="72"/>
+      <c r="H84" s="22"/>
+      <c r="I84" s="27"/>
+      <c r="J84" s="21"/>
+      <c r="K84" s="21"/>
+      <c r="L84" s="21"/>
+      <c r="M84" s="21"/>
+      <c r="N84" s="21"/>
+      <c r="O84" s="21"/>
+      <c r="P84" s="21"/>
+      <c r="Q84" s="21"/>
+    </row>
+    <row r="85" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B85" s="73" t="s">
         <v>116</v>
       </c>
-      <c r="C74" s="72" t="s">
+      <c r="C85" s="72" t="s">
         <v>167</v>
       </c>
     </row>
@@ -4068,12 +4806,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4241,15 +4976,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D8B9148-C797-4C6B-A280-0738F64421E7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F18C333-41DD-4AE5-A5E3-DF6F4E4DF526}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="ac7999f6-dd20-429f-9c50-d27a0c8de317"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4273,17 +5019,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F18C333-41DD-4AE5-A5E3-DF6F4E4DF526}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D8B9148-C797-4C6B-A280-0738F64421E7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="ac7999f6-dd20-429f-9c50-d27a0c8de317"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>